<commit_message>
Changes to WCF Notes
</commit_message>
<xml_diff>
--- a/Database/ADO.Net.xlsx
+++ b/Database/ADO.Net.xlsx
@@ -819,7 +819,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -827,16 +827,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1140,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,30 +1289,38 @@
         <v>21</v>
       </c>
     </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
@@ -1227,10 +1331,11 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D12" t="s">
@@ -1241,18 +1346,20 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
@@ -1263,61 +1370,78 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="8" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+    </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+    <row r="21" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="13" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="25" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="13" t="s">
         <v>39</v>
       </c>
       <c r="E25" s="2" t="s">

</xml_diff>